<commit_message>
Edited to include the non-proposal links
</commit_message>
<xml_diff>
--- a/data_extracts/output_page_consolidated_1to8.xlsx
+++ b/data_extracts/output_page_consolidated_1to8.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\Upwork Project\Messari Selenium\data_extracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC413B08-AC56-4044-97E2-81BF513F2DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463E67C1-2FF5-41AF-95D3-146AE5503DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="proposal_extract_list" sheetId="4" r:id="rId1"/>
-    <sheet name="Extract_Cons_22Jun2023" sheetId="1" r:id="rId2"/>
-    <sheet name="Top 50 DAOs" sheetId="3" r:id="rId3"/>
-    <sheet name="Extract_cons_wkg" sheetId="2" r:id="rId4"/>
+    <sheet name="proposal_extract_list (2)" sheetId="5" r:id="rId1"/>
+    <sheet name="proposal_extract_list" sheetId="4" r:id="rId2"/>
+    <sheet name="Extract_Cons_22Jun2023" sheetId="1" r:id="rId3"/>
+    <sheet name="Top 50 DAOs" sheetId="3" r:id="rId4"/>
+    <sheet name="Extract_cons_wkg" sheetId="2" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Extract_Cons_22Jun2023!$A$1:$S$885</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">proposal_extract_list!$A$1:$C$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Top 50 DAOs'!$B$2:$E$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Extract_Cons_22Jun2023!$A$1:$S$885</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">proposal_extract_list!$A$1:$C$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'proposal_extract_list (2)'!$A$1:$C$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Top 50 DAOs'!$B$2:$E$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11158" uniqueCount="3211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11197" uniqueCount="3211">
   <si>
     <t>coin_name</t>
   </si>
@@ -10529,14 +10531,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F08D606-C7B7-4DA4-A680-C60692EC0B04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C40266-C819-446B-B323-92754D33E619}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10877,6 +10879,258 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F08D606-C7B7-4DA4-A680-C60692EC0B04}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>901</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1879</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>1993</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>2861</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>2862</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19,[1]Datasheet!$C$2:$D$52,2,0)</f>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C19" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S885"/>
@@ -49257,7 +49511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F4A126-19F6-4028-8BCC-701C009A0ACE}">
   <sheetPr filterMode="1"/>
   <dimension ref="B2:E52"/>
@@ -50044,7 +50298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949EEFB6-CB84-4C7F-A741-05A17F7BA944}">
   <dimension ref="A1:P899"/>
   <sheetViews>

</xml_diff>